<commit_message>
Update data.xlsx - 2025-06-05 12:57:46
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shrey\LOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E073C3-94D2-43B6-B3EA-6CF35F6309F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804A8594-8EA3-473C-9B67-69366F099F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48C00C52-6077-402A-B1B8-B4556E09BA5A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11197" uniqueCount="2574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11201" uniqueCount="2576">
   <si>
     <t>ASSOCIATE NAME</t>
   </si>
@@ -7756,6 +7756,12 @@
   </si>
   <si>
     <t>BHUPAL SINGH</t>
+  </si>
+  <si>
+    <t>SIM00414243</t>
+  </si>
+  <si>
+    <t>SNF/45</t>
   </si>
 </sst>
 </file>
@@ -8513,7 +8519,7 @@
   <dimension ref="A1:F3176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8586,14 +8592,24 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>2574</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>2575</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">

</xml_diff>